<commit_message>
added plots Fig1 and Fig3
</commit_message>
<xml_diff>
--- a/benchmarks/results/plots/results-Fig2.xlsx
+++ b/benchmarks/results/plots/results-Fig2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J389"/>
+  <dimension ref="A1:J421"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13674,6 +13674,1094 @@
         <v>39.79164769683307</v>
       </c>
     </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B390" t="n">
+        <v>500</v>
+      </c>
+      <c r="C390" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D390" t="n">
+        <v>0</v>
+      </c>
+      <c r="E390" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F390" t="n">
+        <v>47.97993275550777</v>
+      </c>
+      <c r="G390" t="n">
+        <v>1056.614746349956</v>
+      </c>
+      <c r="H390" t="n">
+        <v>28.32741093155056</v>
+      </c>
+      <c r="I390" t="n">
+        <v>9.062060965211266</v>
+      </c>
+      <c r="J390" t="n">
+        <v>28.71458278916847</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B391" t="n">
+        <v>65</v>
+      </c>
+      <c r="C391" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D391" t="n">
+        <v>0</v>
+      </c>
+      <c r="E391" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F391" t="n">
+        <v>49.65609781879013</v>
+      </c>
+      <c r="G391" t="n">
+        <v>1622.896866179913</v>
+      </c>
+      <c r="H391" t="n">
+        <v>45.73203552001451</v>
+      </c>
+      <c r="I391" t="n">
+        <v>7.385895901928905</v>
+      </c>
+      <c r="J391" t="n">
+        <v>11.30995820070452</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B392" t="n">
+        <v>580</v>
+      </c>
+      <c r="C392" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D392" t="n">
+        <v>0</v>
+      </c>
+      <c r="E392" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F392" t="n">
+        <v>47.11642464565518</v>
+      </c>
+      <c r="G392" t="n">
+        <v>1013.447515844847</v>
+      </c>
+      <c r="H392" t="n">
+        <v>25.25085120935917</v>
+      </c>
+      <c r="I392" t="n">
+        <v>9.925569075063855</v>
+      </c>
+      <c r="J392" t="n">
+        <v>31.79114251135987</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B393" t="n">
+        <v>60</v>
+      </c>
+      <c r="C393" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D393" t="n">
+        <v>0</v>
+      </c>
+      <c r="E393" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F393" t="n">
+        <v>50.08872597113812</v>
+      </c>
+      <c r="G393" t="n">
+        <v>1809.243007695047</v>
+      </c>
+      <c r="H393" t="n">
+        <v>46.05060087590582</v>
+      </c>
+      <c r="I393" t="n">
+        <v>6.953267749580917</v>
+      </c>
+      <c r="J393" t="n">
+        <v>10.99139284481321</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B394" t="n">
+        <v>420</v>
+      </c>
+      <c r="C394" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D394" t="n">
+        <v>0</v>
+      </c>
+      <c r="E394" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F394" t="n">
+        <v>48.1874030872552</v>
+      </c>
+      <c r="G394" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H394" t="n">
+        <v>31.50180904133441</v>
+      </c>
+      <c r="I394" t="n">
+        <v>8.854590633463836</v>
+      </c>
+      <c r="J394" t="n">
+        <v>25.54018467938462</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B395" t="n">
+        <v>3</v>
+      </c>
+      <c r="C395" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D395" t="n">
+        <v>0</v>
+      </c>
+      <c r="E395" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F395" t="n">
+        <v>53.87595673098347</v>
+      </c>
+      <c r="G395" t="n">
+        <v>10385.36486245873</v>
+      </c>
+      <c r="H395" t="n">
+        <v>52.71698023374482</v>
+      </c>
+      <c r="I395" t="n">
+        <v>3.166036989735566</v>
+      </c>
+      <c r="J395" t="n">
+        <v>4.325013486974214</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B396" t="n">
+        <v>1</v>
+      </c>
+      <c r="C396" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D396" t="n">
+        <v>0</v>
+      </c>
+      <c r="E396" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F396" t="n">
+        <v>54.58431692148883</v>
+      </c>
+      <c r="G396" t="n">
+        <v>21741.68594864994</v>
+      </c>
+      <c r="H396" t="n">
+        <v>53.77554729363442</v>
+      </c>
+      <c r="I396" t="n">
+        <v>2.457676799230207</v>
+      </c>
+      <c r="J396" t="n">
+        <v>3.266446427084617</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B397" t="n">
+        <v>8</v>
+      </c>
+      <c r="C397" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D397" t="n">
+        <v>0</v>
+      </c>
+      <c r="E397" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F397" t="n">
+        <v>53.65701634015197</v>
+      </c>
+      <c r="G397" t="n">
+        <v>8747.874059747004</v>
+      </c>
+      <c r="H397" t="n">
+        <v>51.05371690347397</v>
+      </c>
+      <c r="I397" t="n">
+        <v>3.384977380567065</v>
+      </c>
+      <c r="J397" t="n">
+        <v>5.988276817245065</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B398" t="n">
+        <v>6</v>
+      </c>
+      <c r="C398" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D398" t="n">
+        <v>0</v>
+      </c>
+      <c r="E398" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F398" t="n">
+        <v>53.71567707197253</v>
+      </c>
+      <c r="G398" t="n">
+        <v>9009.80646665667</v>
+      </c>
+      <c r="H398" t="n">
+        <v>51.70474070568839</v>
+      </c>
+      <c r="I398" t="n">
+        <v>3.326316648746506</v>
+      </c>
+      <c r="J398" t="n">
+        <v>5.337253015030647</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B399" t="n">
+        <v>610</v>
+      </c>
+      <c r="C399" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D399" t="n">
+        <v>0</v>
+      </c>
+      <c r="E399" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F399" t="n">
+        <v>46.86861350038294</v>
+      </c>
+      <c r="G399" t="n">
+        <v>1002.245676223203</v>
+      </c>
+      <c r="H399" t="n">
+        <v>24.12624764429263</v>
+      </c>
+      <c r="I399" t="n">
+        <v>10.17338022033609</v>
+      </c>
+      <c r="J399" t="n">
+        <v>32.9157460764264</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B400" t="n">
+        <v>1e+16</v>
+      </c>
+      <c r="C400" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D400" t="n">
+        <v>0</v>
+      </c>
+      <c r="E400" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F400" t="n">
+        <v>29.326573568</v>
+      </c>
+      <c r="G400" t="n">
+        <v>889.6259531912921</v>
+      </c>
+      <c r="H400" t="n">
+        <v>-330932225215385.4</v>
+      </c>
+      <c r="I400" t="n">
+        <v>27.71542015271903</v>
+      </c>
+      <c r="J400" t="n">
+        <v>330932225215442.4</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B401" t="n">
+        <v>630</v>
+      </c>
+      <c r="C401" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D401" t="n">
+        <v>0</v>
+      </c>
+      <c r="E401" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F401" t="n">
+        <v>46.70547397112593</v>
+      </c>
+      <c r="G401" t="n">
+        <v>995.1507456279003</v>
+      </c>
+      <c r="H401" t="n">
+        <v>23.38372923321111</v>
+      </c>
+      <c r="I401" t="n">
+        <v>10.3365197495931</v>
+      </c>
+      <c r="J401" t="n">
+        <v>33.65826448750792</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B402" t="n">
+        <v>620</v>
+      </c>
+      <c r="C402" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D402" t="n">
+        <v>0</v>
+      </c>
+      <c r="E402" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F402" t="n">
+        <v>46.78588689719382</v>
+      </c>
+      <c r="G402" t="n">
+        <v>998.6204177211238</v>
+      </c>
+      <c r="H402" t="n">
+        <v>23.75430615319304</v>
+      </c>
+      <c r="I402" t="n">
+        <v>10.25610682352522</v>
+      </c>
+      <c r="J402" t="n">
+        <v>33.28768756752599</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B403" t="n">
+        <v>390</v>
+      </c>
+      <c r="C403" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D403" t="n">
+        <v>0</v>
+      </c>
+      <c r="E403" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F403" t="n">
+        <v>48.18740308725521</v>
+      </c>
+      <c r="G403" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H403" t="n">
+        <v>32.69363718747162</v>
+      </c>
+      <c r="I403" t="n">
+        <v>8.854590633463822</v>
+      </c>
+      <c r="J403" t="n">
+        <v>24.34835653324741</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B404" t="n">
+        <v>4</v>
+      </c>
+      <c r="C404" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D404" t="n">
+        <v>0</v>
+      </c>
+      <c r="E404" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F404" t="n">
+        <v>53.80672461550006</v>
+      </c>
+      <c r="G404" t="n">
+        <v>9519.301348137373</v>
+      </c>
+      <c r="H404" t="n">
+        <v>52.39028950978646</v>
+      </c>
+      <c r="I404" t="n">
+        <v>3.235269105218975</v>
+      </c>
+      <c r="J404" t="n">
+        <v>4.651704210932571</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B405" t="n">
+        <v>410</v>
+      </c>
+      <c r="C405" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D405" t="n">
+        <v>0</v>
+      </c>
+      <c r="E405" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F405" t="n">
+        <v>48.1874030872552</v>
+      </c>
+      <c r="G405" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H405" t="n">
+        <v>31.89908509004681</v>
+      </c>
+      <c r="I405" t="n">
+        <v>8.854590633463836</v>
+      </c>
+      <c r="J405" t="n">
+        <v>25.14290863067222</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B406" t="n">
+        <v>7</v>
+      </c>
+      <c r="C406" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D406" t="n">
+        <v>0</v>
+      </c>
+      <c r="E406" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F406" t="n">
+        <v>53.49831041749932</v>
+      </c>
+      <c r="G406" t="n">
+        <v>8717.176637523147</v>
+      </c>
+      <c r="H406" t="n">
+        <v>51.22841681071766</v>
+      </c>
+      <c r="I406" t="n">
+        <v>3.543683303219716</v>
+      </c>
+      <c r="J406" t="n">
+        <v>5.813576910001373</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B407" t="n">
+        <v>145</v>
+      </c>
+      <c r="C407" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D407" t="n">
+        <v>0</v>
+      </c>
+      <c r="E407" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F407" t="n">
+        <v>48.18740308725521</v>
+      </c>
+      <c r="G407" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H407" t="n">
+        <v>42.42690038092541</v>
+      </c>
+      <c r="I407" t="n">
+        <v>8.854590633463822</v>
+      </c>
+      <c r="J407" t="n">
+        <v>14.61509333979362</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B408" t="n">
+        <v>740</v>
+      </c>
+      <c r="C408" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D408" t="n">
+        <v>0</v>
+      </c>
+      <c r="E408" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F408" t="n">
+        <v>45.88276327422266</v>
+      </c>
+      <c r="G408" t="n">
+        <v>962.6327851215189</v>
+      </c>
+      <c r="H408" t="n">
+        <v>19.38409894321065</v>
+      </c>
+      <c r="I408" t="n">
+        <v>11.15923044649637</v>
+      </c>
+      <c r="J408" t="n">
+        <v>37.65789477750839</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B409" t="n">
+        <v>370</v>
+      </c>
+      <c r="C409" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D409" t="n">
+        <v>0</v>
+      </c>
+      <c r="E409" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F409" t="n">
+        <v>48.18740308725521</v>
+      </c>
+      <c r="G409" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H409" t="n">
+        <v>33.48818928489641</v>
+      </c>
+      <c r="I409" t="n">
+        <v>8.854590633463822</v>
+      </c>
+      <c r="J409" t="n">
+        <v>23.55380443582263</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B410" t="n">
+        <v>600</v>
+      </c>
+      <c r="C410" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D410" t="n">
+        <v>0</v>
+      </c>
+      <c r="E410" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F410" t="n">
+        <v>46.95379500295929</v>
+      </c>
+      <c r="G410" t="n">
+        <v>1006.038007987869</v>
+      </c>
+      <c r="H410" t="n">
+        <v>24.4996121787907</v>
+      </c>
+      <c r="I410" t="n">
+        <v>10.08819871775975</v>
+      </c>
+      <c r="J410" t="n">
+        <v>32.54238154192834</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B411" t="n">
+        <v>680</v>
+      </c>
+      <c r="C411" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D411" t="n">
+        <v>0</v>
+      </c>
+      <c r="E411" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F411" t="n">
+        <v>46.35242482763016</v>
+      </c>
+      <c r="G411" t="n">
+        <v>980.5402281018844</v>
+      </c>
+      <c r="H411" t="n">
+        <v>21.54932598189934</v>
+      </c>
+      <c r="I411" t="n">
+        <v>10.68956889308888</v>
+      </c>
+      <c r="J411" t="n">
+        <v>35.49266773881969</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B412" t="n">
+        <v>430</v>
+      </c>
+      <c r="C412" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D412" t="n">
+        <v>0</v>
+      </c>
+      <c r="E412" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F412" t="n">
+        <v>48.18740308725521</v>
+      </c>
+      <c r="G412" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H412" t="n">
+        <v>31.10453299262203</v>
+      </c>
+      <c r="I412" t="n">
+        <v>8.854590633463822</v>
+      </c>
+      <c r="J412" t="n">
+        <v>25.937460728097</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B413" t="n">
+        <v>730</v>
+      </c>
+      <c r="C413" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D413" t="n">
+        <v>0</v>
+      </c>
+      <c r="E413" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F413" t="n">
+        <v>45.95906874431417</v>
+      </c>
+      <c r="G413" t="n">
+        <v>965.4264344845503</v>
+      </c>
+      <c r="H413" t="n">
+        <v>19.74263210790998</v>
+      </c>
+      <c r="I413" t="n">
+        <v>11.08292497640486</v>
+      </c>
+      <c r="J413" t="n">
+        <v>37.29936161280905</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B414" t="n">
+        <v>165</v>
+      </c>
+      <c r="C414" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D414" t="n">
+        <v>0</v>
+      </c>
+      <c r="E414" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F414" t="n">
+        <v>48.18740308725522</v>
+      </c>
+      <c r="G414" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H414" t="n">
+        <v>41.63234828350063</v>
+      </c>
+      <c r="I414" t="n">
+        <v>8.854590633463815</v>
+      </c>
+      <c r="J414" t="n">
+        <v>15.4096454372184</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B415" t="n">
+        <v>400</v>
+      </c>
+      <c r="C415" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D415" t="n">
+        <v>0</v>
+      </c>
+      <c r="E415" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F415" t="n">
+        <v>48.18740308725521</v>
+      </c>
+      <c r="G415" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H415" t="n">
+        <v>32.29636113875923</v>
+      </c>
+      <c r="I415" t="n">
+        <v>8.854590633463822</v>
+      </c>
+      <c r="J415" t="n">
+        <v>24.7456325819598</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B416" t="n">
+        <v>640</v>
+      </c>
+      <c r="C416" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D416" t="n">
+        <v>0</v>
+      </c>
+      <c r="E416" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F416" t="n">
+        <v>46.62724313095844</v>
+      </c>
+      <c r="G416" t="n">
+        <v>991.8261512019781</v>
+      </c>
+      <c r="H416" t="n">
+        <v>23.01446184881642</v>
+      </c>
+      <c r="I416" t="n">
+        <v>10.41475058976059</v>
+      </c>
+      <c r="J416" t="n">
+        <v>34.02753187190261</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B417" t="n">
+        <v>75</v>
+      </c>
+      <c r="C417" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D417" t="n">
+        <v>0</v>
+      </c>
+      <c r="E417" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F417" t="n">
+        <v>48.1874030872552</v>
+      </c>
+      <c r="G417" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H417" t="n">
+        <v>45.2078327219122</v>
+      </c>
+      <c r="I417" t="n">
+        <v>8.854590633463836</v>
+      </c>
+      <c r="J417" t="n">
+        <v>11.83416099880684</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B418" t="n">
+        <v>55</v>
+      </c>
+      <c r="C418" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D418" t="n">
+        <v>0</v>
+      </c>
+      <c r="E418" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F418" t="n">
+        <v>50.59192765071704</v>
+      </c>
+      <c r="G418" t="n">
+        <v>2044.961440343802</v>
+      </c>
+      <c r="H418" t="n">
+        <v>46.40804564246646</v>
+      </c>
+      <c r="I418" t="n">
+        <v>6.450066070001995</v>
+      </c>
+      <c r="J418" t="n">
+        <v>10.63394807825257</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B419" t="n">
+        <v>125</v>
+      </c>
+      <c r="C419" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D419" t="n">
+        <v>0</v>
+      </c>
+      <c r="E419" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F419" t="n">
+        <v>48.18740308725521</v>
+      </c>
+      <c r="G419" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H419" t="n">
+        <v>43.22145247835022</v>
+      </c>
+      <c r="I419" t="n">
+        <v>8.854590633463822</v>
+      </c>
+      <c r="J419" t="n">
+        <v>13.82054124236881</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B420" t="n">
+        <v>105</v>
+      </c>
+      <c r="C420" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D420" t="n">
+        <v>0</v>
+      </c>
+      <c r="E420" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F420" t="n">
+        <v>48.1874030872552</v>
+      </c>
+      <c r="G420" t="n">
+        <v>1067.974215221202</v>
+      </c>
+      <c r="H420" t="n">
+        <v>44.016004575775</v>
+      </c>
+      <c r="I420" t="n">
+        <v>8.854590633463836</v>
+      </c>
+      <c r="J420" t="n">
+        <v>13.02598914494403</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=time_gradient_targetGroups=False_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B421" t="n">
+        <v>9</v>
+      </c>
+      <c r="C421" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D421" t="n">
+        <v>0</v>
+      </c>
+      <c r="E421" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F421" t="n">
+        <v>53.61810498285629</v>
+      </c>
+      <c r="G421" t="n">
+        <v>8596.69973313073</v>
+      </c>
+      <c r="H421" t="n">
+        <v>50.74000496139278</v>
+      </c>
+      <c r="I421" t="n">
+        <v>3.423888737862747</v>
+      </c>
+      <c r="J421" t="n">
+        <v>6.301988759326257</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>